<commit_message>
set up reverse solving for e-motor. cleaning up variable names for hybrid nacelle
</commit_message>
<xml_diff>
--- a/openconcept/propulsion/empirical_data/H3X_HPDM-XXXX_1MW.xlsx
+++ b/openconcept/propulsion/empirical_data/H3X_HPDM-XXXX_1MW.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\lucstmich\repos\aircraft_performance\models\apolo\PerfData\electricMotor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eosaircraft-my.sharepoint.com/personal/aamos_eos_aero/Documents/Documents/GitHub/openconcept/openconcept/propulsion/empirical_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47881747-CEB4-4823-B068-FF5651E86818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{47881747-CEB4-4823-B068-FF5651E86818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB090BB3-AC8A-496B-B9C7-222BC678A2A2}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,16 +475,16 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="10.109375" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -501,7 +501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>450</v>
       </c>
@@ -520,7 +520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>450</v>
       </c>
@@ -539,7 +539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>450</v>
       </c>
@@ -558,7 +558,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>450</v>
       </c>
@@ -577,7 +577,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>450</v>
       </c>
@@ -596,7 +596,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>450</v>
       </c>
@@ -615,7 +615,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>450</v>
       </c>
@@ -634,7 +634,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>450</v>
       </c>
@@ -652,7 +652,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>450</v>
       </c>
@@ -671,7 +671,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>450</v>
       </c>
@@ -689,7 +689,7 @@
         <v>1865</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>550</v>
       </c>
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>550</v>
       </c>
@@ -727,7 +727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>550</v>
       </c>
@@ -746,7 +746,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>550</v>
       </c>
@@ -765,7 +765,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>550</v>
       </c>
@@ -784,7 +784,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>550</v>
       </c>
@@ -803,7 +803,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>550</v>
       </c>
@@ -822,7 +822,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>550</v>
       </c>
@@ -840,7 +840,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>550</v>
       </c>
@@ -859,7 +859,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>550</v>
       </c>
@@ -877,7 +877,7 @@
         <v>1865</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>800</v>
       </c>
@@ -896,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>800</v>
       </c>
@@ -915,7 +915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>800</v>
       </c>
@@ -934,7 +934,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>800</v>
       </c>
@@ -953,7 +953,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>800</v>
       </c>
@@ -972,7 +972,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>800</v>
       </c>
@@ -991,7 +991,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>800</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>800</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>800</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>800</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>1865</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>900</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>900</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>900</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>900</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>900</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>900</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>900</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>900</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>900</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>900</v>
       </c>

</xml_diff>